<commit_message>
Trådløs kommunikations protokol mm.
</commit_message>
<xml_diff>
--- a/Design og implementering/Body SW/SensorConfig.xlsx
+++ b/Design og implementering/Body SW/SensorConfig.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
   <si>
     <t>SensorID</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>PRX4_ID</t>
-  </si>
-  <si>
-    <t>BluetoothArray</t>
   </si>
 </sst>
 </file>
@@ -162,10 +159,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G18"/>
+  <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F18" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -472,10 +468,9 @@
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
+    <row r="2" spans="2:6">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,11 +486,8 @@
       <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7">
+    </row>
+    <row r="3" spans="2:6">
       <c r="B3" s="1">
         <v>0</v>
       </c>
@@ -511,11 +503,8 @@
       <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7">
+    </row>
+    <row r="4" spans="2:6">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -531,11 +520,8 @@
       <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7">
+    </row>
+    <row r="5" spans="2:6">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -551,11 +537,8 @@
       <c r="F5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7">
+    </row>
+    <row r="6" spans="2:6">
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -571,11 +554,8 @@
       <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7">
+    </row>
+    <row r="7" spans="2:6">
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -591,11 +571,8 @@
       <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7">
+    </row>
+    <row r="8" spans="2:6">
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -611,11 +588,8 @@
       <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7">
+    </row>
+    <row r="9" spans="2:6">
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -631,11 +605,8 @@
       <c r="F9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7">
+    </row>
+    <row r="10" spans="2:6">
       <c r="B10" s="1">
         <v>7</v>
       </c>
@@ -651,11 +622,8 @@
       <c r="F10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7">
+    </row>
+    <row r="11" spans="2:6">
       <c r="B11" s="1">
         <v>8</v>
       </c>
@@ -671,11 +639,8 @@
       <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7">
+    </row>
+    <row r="12" spans="2:6">
       <c r="B12" s="1">
         <v>9</v>
       </c>
@@ -691,11 +656,8 @@
       <c r="F12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7">
+    </row>
+    <row r="13" spans="2:6">
       <c r="B13" s="1">
         <v>10</v>
       </c>
@@ -711,11 +673,8 @@
       <c r="F13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="1">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7">
+    </row>
+    <row r="14" spans="2:6">
       <c r="B14" s="1">
         <v>11</v>
       </c>
@@ -731,11 +690,8 @@
       <c r="F14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="1">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7">
+    </row>
+    <row r="15" spans="2:6">
       <c r="B15" s="1">
         <v>12</v>
       </c>
@@ -751,11 +707,8 @@
       <c r="F15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="1">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7">
+    </row>
+    <row r="16" spans="2:6">
       <c r="B16" s="1">
         <v>13</v>
       </c>
@@ -771,11 +724,8 @@
       <c r="F16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="1">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7">
+    </row>
+    <row r="17" spans="2:6">
       <c r="B17" s="1">
         <v>14</v>
       </c>
@@ -791,11 +741,8 @@
       <c r="F17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="1">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7">
+    </row>
+    <row r="18" spans="2:6">
       <c r="B18" s="1">
         <v>15</v>
       </c>
@@ -810,9 +757,6 @@
       </c>
       <c r="F18" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="G18" s="1">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>